<commit_message>
Just needs to be printed out!
</commit_message>
<xml_diff>
--- a/Projects/GabrielAnderson_P2V2/Expected InputOutput.xlsx
+++ b/Projects/GabrielAnderson_P2V2/Expected InputOutput.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="659" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,12 +17,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
-  <si>
-    <t>First Student (1)</t>
-  </si>
-  <si>
-    <t>First Student (2)</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
+  <si>
+    <t>Student Object</t>
+  </si>
+  <si>
+    <t>firstStudent (run 1)</t>
+  </si>
+  <si>
+    <t>firstStudent (run 2)</t>
+  </si>
+  <si>
+    <t>secondStudent</t>
+  </si>
+  <si>
+    <t>thirdStudent</t>
+  </si>
+  <si>
+    <t>fourthStudent</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>First Student</t>
   </si>
   <si>
     <t>Second Student</t>
@@ -31,6 +49,9 @@
     <t>Third Student</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>Scores</t>
   </si>
   <si>
@@ -43,9 +64,6 @@
     <t>Number of quizzes</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>Total Quiz Score</t>
   </si>
   <si>
@@ -65,6 +83,21 @@
   </si>
   <si>
     <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>A's</t>
+  </si>
+  <si>
+    <t>B's</t>
+  </si>
+  <si>
+    <t>C's</t>
+  </si>
+  <si>
+    <t>D's</t>
+  </si>
+  <si>
+    <t>F's</t>
   </si>
 </sst>
 </file>
@@ -74,7 +107,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -96,12 +129,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -146,24 +173,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -182,13 +201,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -198,110 +217,126 @@
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="17.004048582996"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.8542510121457"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.331983805668"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.8704453441296"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.5587044534413"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.5748987854251"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="D2" s="2" t="n">
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>79</v>
+      </c>
+      <c r="D3" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="E2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
-      <c r="B3" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="D3" s="2" t="n">
+      <c r="E3" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="2"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1"/>
+      <c r="B4" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>80</v>
+      </c>
+      <c r="D4" s="2" t="n">
         <v>15.77</v>
-      </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
-      <c r="B4" s="2" t="n">
-        <v>82</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>14</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>101</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3"/>
+      <c r="A5" s="1"/>
       <c r="B5" s="2" t="n">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>92</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>5</v>
+        <v>89</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>101</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
+      <c r="A6" s="1"/>
       <c r="B6" s="2" t="n">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2" t="n">
+        <v>70</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
+      <c r="A8" s="1"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -309,7 +344,7 @@
       <c r="F8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3"/>
+      <c r="A9" s="1"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -317,167 +352,292 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <f aca="false">COUNT(B2:B8)</f>
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <f aca="false">COUNT(B3:B9)</f>
         <v>5</v>
       </c>
-      <c r="C10" s="2" t="n">
-        <f aca="false">COUNT(B2:B6,C2:C6)</f>
-        <v>10</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <f aca="false">COUNT(E2:E8)</f>
+      <c r="C11" s="2" t="n">
+        <f aca="false">COUNT(B3:B7,C3:C7)</f>
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="2" t="n">
+        <f aca="false">COUNT(E3:E9)</f>
         <v>1</v>
       </c>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <f aca="false">SUM(B2:B8)</f>
-        <v>372</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <f aca="false">SUM(C2:C6,B2:B6)</f>
-        <v>771</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2" t="n">
-        <f aca="false">MIN(B2:B6)</f>
-        <v>0</v>
+        <f aca="false">SUM(B3:B9)</f>
+        <v>258</v>
       </c>
       <c r="C12" s="2" t="n">
-        <f aca="false">MIN(B2:B6,C2:C6)</f>
-        <v>0</v>
+        <f aca="false">SUM(C3:C7,B3:B7)</f>
+        <v>696</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2" t="n">
-        <f aca="false">MAX(B2:B6)</f>
-        <v>100</v>
+        <f aca="false">MIN(B3:B7)</f>
+        <v>0</v>
       </c>
       <c r="C13" s="2" t="n">
-        <f aca="false">MAX(B2:B6,C2:C6)</f>
-        <v>100</v>
+        <f aca="false">MIN(B3:B7,C3:C7)</f>
+        <v>0</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>12</v>
+      <c r="A14" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="B14" s="2" t="n">
-        <f aca="false">AVERAGE(B2:B8)</f>
-        <v>74.4</v>
+        <f aca="false">MAX(B3:B7)</f>
+        <v>70</v>
       </c>
       <c r="C14" s="2" t="n">
-        <f aca="false">AVERAGE(B1:B6,C2:C6)</f>
-        <v>77.1</v>
+        <f aca="false">MAX(B3:B7,C3:C7)</f>
+        <v>100</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2" t="n">
-        <f aca="false">AVERAGE(E2)</f>
-        <v>0</v>
-      </c>
-      <c r="F14" s="2"/>
+        <v>1</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2" t="n">
-        <f aca="false">SUMSQ(B2:B6)</f>
-        <v>34806</v>
+        <f aca="false">AVERAGE(B3:B9)</f>
+        <v>51.6</v>
       </c>
       <c r="C15" s="2" t="n">
-        <f aca="false">SUMSQ(B2:B6,C2:C6)</f>
-        <v>72115</v>
+        <f aca="false">AVERAGE(B2:B7,C3:C7)</f>
+        <v>69.6</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="n">
-        <f aca="false">SUMSQ(E2)</f>
-        <v>0</v>
-      </c>
-      <c r="F15" s="2"/>
+        <f aca="false">AVERAGE(E3)</f>
+        <v>0</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2" t="n">
-        <f aca="false">VAR(B2:B6)</f>
-        <v>1782.3</v>
+        <f aca="false">SUMSQ(B3:B7)</f>
+        <v>16742</v>
       </c>
       <c r="C16" s="2" t="n">
-        <f aca="false">VAR(B2:B6,C2:C6)</f>
-        <v>1407.87777777778</v>
+        <f aca="false">SUMSQ(B3:B7,C3:C7)</f>
+        <v>55404</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" s="2"/>
+        <f aca="false">SUMSQ(E3)</f>
+        <v>0</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2" t="n">
-        <f aca="false">STDEV(B2:B6)</f>
-        <v>42.2172950341445</v>
+        <f aca="false">VAR(B3:B7)</f>
+        <v>857.3</v>
       </c>
       <c r="C17" s="2" t="n">
-        <f aca="false">STDEV(B2:B6,C2:C6)</f>
-        <v>37.5216974266594</v>
+        <f aca="false">VAR(B3:B7,C3:C7)</f>
+        <v>773.6</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="F17" s="2"/>
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <f aca="false">STDEV(B3:B7)</f>
+        <v>29.2796857906638</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <f aca="false">STDEV(B3:B7,C3:C7)</f>
+        <v>27.8136657059079</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -493,7 +653,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
@@ -520,7 +680,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
-    <tabColor rgb="00FFFFFF"/>
+    <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>

</xml_diff>